<commit_message>
Question 3 Completed with data, Question 1 part 2 completed
</commit_message>
<xml_diff>
--- a/结果表/结果表2-预测结果表.xlsx
+++ b/结果表/结果表2-预测结果表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziyi_wang/Documents/Codes/PY/Modelcon/结果表/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC33F2D-9ABD-3546-B78C-12ED6FBBD80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643B6D26-AB23-EF4E-A05B-4BF5BD8C3B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -729,7 +729,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A1093" workbookViewId="0">
+      <selection activeCell="E1022" sqref="E1022"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>